<commit_message>
changed default config for separate business output to TRUE
</commit_message>
<xml_diff>
--- a/app/gg_fare_input.xlsx
+++ b/app/gg_fare_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pingsays/git/farefiling/app/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4692A05B-C3C7-4C4E-BB73-5B9312A5AE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64802316-7BF7-924A-9A09-34889388302D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="input" sheetId="1" r:id="rId1"/>
@@ -255,9 +255,6 @@
   </cellStyles>
   <dxfs count="25">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center"/>
     </dxf>
     <dxf>
@@ -266,6 +263,9 @@
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
       <alignment horizontal="center" vertical="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center"/>
@@ -401,10 +401,10 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="weekday" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="oneway" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="oneway_multiplier" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="weekend_surcharge" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="oneway_mapping" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="oneway" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="oneway_multiplier" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="weekend_surcharge" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="oneway_mapping" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2590,7 +2590,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -2702,7 +2702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D86AFF6-317A-544C-9C0F-542021E4A510}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2718,7 +2718,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>